<commit_message>
Adding project diary and project notes
</commit_message>
<xml_diff>
--- a/Documents/Team Details.xlsx
+++ b/Documents/Team Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AnalysisofRubiksCubeSolvingAlgorithm\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6509B341-A9DC-4EA7-911A-ED7248DC2D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7641A5A0-E361-4EDD-932D-A5E1D9F0973F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>

</xml_diff>